<commit_message>
Reorder supervision by year
</commit_message>
<xml_diff>
--- a/data/supervision_pos_en.xlsx
+++ b/data/supervision_pos_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\JDL_CV\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853D1FAA-54FB-450E-B58E-002344627DD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F390701A-49AC-47FA-AA22-DC7DF71667C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="supervision" sheetId="1" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>\href{https://www.uel.ac.uk/}{U. of East London}, UK</t>
   </si>
   <si>
-    <t>Supervised together with  Alicia Salvador</t>
-  </si>
-  <si>
     <t>Supervised together with Lisa Chiara Fellin</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>Research project \textbf{\textit{(Distinction)}}: \textit{Sexy Chat: Mate-Choice Preferences for Speech Content in the Absence of Auditory Cues}</t>
+  </si>
+  <si>
+    <t>Supervised together with Alicia Salvador</t>
   </si>
 </sst>
 </file>
@@ -969,7 +969,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="58.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1012,7 +1012,7 @@
         <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1038,7 +1038,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1047,27 +1047,27 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1076,30 +1076,30 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>